<commit_message>
Added 24 hour prediction
</commit_message>
<xml_diff>
--- a/Machine_learning/Electricity_demand_prediction/Data_electricity/Hourly_Active_power_04_11_23.xlsx
+++ b/Machine_learning/Electricity_demand_prediction/Data_electricity/Hourly_Active_power_04_11_23.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dehtd\Desktop\Repositories\wolfheze-git\Machine_learning\Data_electricity\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dehtd\Desktop\Repositories\wolfheze-git\Machine_learning\Electricity_demand_prediction\Data_electricity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385535B7-E850-426D-B721-B07F73F128BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1578A5F8-634E-4D79-9338-829880EF23E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4445" uniqueCount="4445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4447" uniqueCount="4447">
   <si>
     <t>time</t>
   </si>
@@ -13371,6 +13371,12 @@
   </si>
   <si>
     <t>2023-10-31T23:00:00.000+01:00</t>
+  </si>
+  <si>
+    <t>doy</t>
+  </si>
+  <si>
+    <t>weekend</t>
   </si>
 </sst>
 </file>
@@ -14211,10 +14217,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4443"/>
+  <dimension ref="A1:E4443"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4389" workbookViewId="0">
-      <selection activeCell="J4398" sqref="J4398"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14223,7 +14229,7 @@
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -14233,8 +14239,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>4445</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4446</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -14246,7 +14258,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -14258,7 +14270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -14270,7 +14282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -14282,7 +14294,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -14294,7 +14306,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -14306,7 +14318,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -14318,7 +14330,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -14330,7 +14342,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -14342,7 +14354,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -14354,7 +14366,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -14366,7 +14378,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -14378,7 +14390,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -14390,7 +14402,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -14402,7 +14414,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -67544,12 +67556,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2af00115-db01-40d3-bf7a-0579e6c39f03">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d5395088-56a8-456d-897f-05b0b359297f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -67754,20 +67768,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2af00115-db01-40d3-bf7a-0579e6c39f03">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d5395088-56a8-456d-897f-05b0b359297f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8854E42-9379-41A8-89E8-EE251DB94A8B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9069DD32-5287-4535-A833-05D06E7BA9F2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d5395088-56a8-456d-897f-05b0b359297f"/>
+    <ds:schemaRef ds:uri="2af00115-db01-40d3-bf7a-0579e6c39f03"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -67792,18 +67813,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9069DD32-5287-4535-A833-05D06E7BA9F2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8854E42-9379-41A8-89E8-EE251DB94A8B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d5395088-56a8-456d-897f-05b0b359297f"/>
-    <ds:schemaRef ds:uri="2af00115-db01-40d3-bf7a-0579e6c39f03"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>